<commit_message>
commit adjust thfyjs details (#3130)
Co-authored-by: 汤永靖 <tangyongjing@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/DesignData/SmokeProofScenario.xlsx
+++ b/AutoLoader/Contents/Support/DesignData/SmokeProofScenario.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BaiduNetdiskDownload\产品开发\01_暖通\02_防烟计算（消防加压送风）\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Autodesk\ApplicationPlugins\ThMEPPlugin.bundle\Contents\Support\DesignData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="782" activeTab="6"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="782"/>
   </bookViews>
   <sheets>
     <sheet name="消防电梯前室" sheetId="1" r:id="rId1"/>
@@ -56,18 +56,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="77">
   <si>
     <t>系统名称</t>
-  </si>
-  <si>
-    <t>（风机编号）</t>
-  </si>
-  <si>
-    <t>服务区域</t>
-  </si>
-  <si>
-    <t>最终值：</t>
   </si>
   <si>
     <t>ΔP</t>
@@ -359,18 +350,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（楼梯所在区域）</t>
-  </si>
-  <si>
     <t>楼梯位置</t>
-  </si>
-  <si>
-    <t>风机的“服务区域”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>风机的“风机编号”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
@@ -639,6 +619,14 @@
   </si>
   <si>
     <t>Type_Door_Q1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统计算风量：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>面板输入值“风机编号”</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -837,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -880,15 +868,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -905,6 +884,15 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -915,21 +903,63 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1212,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -1227,98 +1257,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="A1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="28"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="9"/>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="28"/>
+      <c r="A3" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="9"/>
       <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="9"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.25">
+      <c r="A4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="16"/>
       <c r="F4" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="16"/>
       <c r="F5" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="16"/>
-      <c r="F6" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17.25">
-      <c r="A8" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="16"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18">
+      <c r="A6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.25">
+      <c r="A7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="16"/>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="17"/>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D9" s="17"/>
       <c r="F9" s="1" t="s">
@@ -1329,156 +1355,144 @@
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" s="17"/>
       <c r="F10" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="17"/>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="18"/>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="18"/>
       <c r="F12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="18"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="19"/>
       <c r="F13" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="12"/>
       <c r="F14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="12"/>
-      <c r="F15" s="1" t="s">
-        <v>25</v>
+      <c r="F15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="3"/>
-      <c r="B16" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="29"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="25"/>
       <c r="D16" s="12"/>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2"/>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="12"/>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="32"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="F18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="33"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="12"/>
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2"/>
-      <c r="B18" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="12"/>
-      <c r="F18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="32"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="D19" s="12"/>
       <c r="F19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="33"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D20" s="12"/>
       <c r="F20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="34"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="F21" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A19:A21"/>
+  <mergeCells count="14">
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1487,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1500,12 +1514,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="A1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1515,100 +1529,96 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="28"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="9"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="28"/>
+      <c r="A3" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="9"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="9"/>
+    <row r="4" spans="1:8" ht="17.25">
+      <c r="A4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="17.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="16"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="17.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="16"/>
+    <row r="6" spans="1:8" ht="18">
+      <c r="A6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="18">
-      <c r="A7" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="16" t="s">
-        <v>24</v>
-      </c>
+    <row r="7" spans="1:8" ht="17.25">
+      <c r="A7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="17.25">
-      <c r="A8" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="16"/>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="17"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1617,7 +1627,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="1"/>
@@ -1631,26 +1641,26 @@
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="17.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="17"/>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="18"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1659,26 +1669,26 @@
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="17.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1687,154 +1697,139 @@
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="18"/>
+      <c r="A15" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="12"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>25</v>
+      <c r="F17" t="s">
+        <v>20</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="3"/>
-      <c r="B18" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="29"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="25"/>
       <c r="D18" s="12"/>
       <c r="E18" s="1"/>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2"/>
-      <c r="B19" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="28"/>
+      <c r="B19" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="25"/>
       <c r="D19" s="12"/>
       <c r="E19" s="1"/>
-      <c r="F19" t="s">
-        <v>30</v>
+      <c r="F19" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="2"/>
-      <c r="B20" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="28"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="D20" s="12"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="F20" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="32"/>
-      <c r="B21" s="20"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D21" s="12"/>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="33"/>
-      <c r="B22" s="21"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D22" s="12"/>
       <c r="F22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="34"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="F23" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
+  <mergeCells count="14">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1843,10 +1838,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1855,12 +1850,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="A1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1870,100 +1865,96 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="28"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="9"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="28"/>
+      <c r="A3" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="9"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="9"/>
+    <row r="4" spans="1:8" ht="17.25">
+      <c r="A4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="17.25">
-      <c r="A5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="16"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="17.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="16"/>
+    <row r="6" spans="1:8" ht="18">
+      <c r="A6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="18">
-      <c r="A7" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="16" t="s">
-        <v>24</v>
-      </c>
+    <row r="7" spans="1:8" ht="17.25">
+      <c r="A7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="17.25">
-      <c r="A8" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="16"/>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="17"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1972,7 +1963,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="1"/>
@@ -1986,26 +1977,26 @@
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="17.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="17"/>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="18"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -2014,154 +2005,139 @@
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="17.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="18"/>
+    <row r="13" spans="1:8">
+      <c r="A13" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="12"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
-        <v>25</v>
+      <c r="F15" t="s">
+        <v>20</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="3"/>
-      <c r="B16" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="29"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="25"/>
       <c r="D16" s="12"/>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2"/>
-      <c r="B17" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="28"/>
+      <c r="B17" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="25"/>
       <c r="D17" s="12"/>
       <c r="E17" s="1"/>
-      <c r="F17" t="s">
-        <v>30</v>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="2"/>
-      <c r="B18" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="28"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="D18" s="12"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="F18" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="32"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D19" s="12"/>
       <c r="F19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="33"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D20" s="12"/>
       <c r="F20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="34"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="F21" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A6:C6"/>
+  <mergeCells count="14">
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2170,10 +2146,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2184,97 +2160,93 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="30" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="28"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="9"/>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="9"/>
+      <c r="A3" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="10"/>
       <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="10"/>
-      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.25">
+      <c r="A4" s="23" t="s">
         <v>41</v>
       </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="13"/>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="17.25">
-      <c r="A5" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="13"/>
       <c r="F5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18">
+      <c r="A6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="13"/>
       <c r="F6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="13"/>
-      <c r="F7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17.25">
-      <c r="A8" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="13" t="s">
-        <v>24</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.25">
+      <c r="A7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="F8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D9" s="11"/>
       <c r="F9" t="s">
@@ -2285,144 +2257,144 @@
       <c r="A10" s="3"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" s="11"/>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="D11" s="11"/>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="D12" s="11"/>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D13" s="11"/>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="F14" t="s">
-        <v>54</v>
+      <c r="A14" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="14"/>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="14"/>
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="15"/>
       <c r="F15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="31"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="29"/>
       <c r="D16" s="15"/>
-      <c r="F16" s="1" t="s">
-        <v>25</v>
+      <c r="F16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3"/>
       <c r="B17" s="29" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="15"/>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
       <c r="B18" s="29" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="15"/>
       <c r="F18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="29"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="13.9" customHeight="1">
+      <c r="A19" s="32"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="D19" s="15"/>
       <c r="F19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="13.9" customHeight="1">
-      <c r="A20" s="32"/>
-      <c r="B20" s="20"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="33"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D20" s="15"/>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="33"/>
-      <c r="B21" s="21"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D21" s="15"/>
       <c r="F21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="33"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="7" t="s">
-        <v>76</v>
+      <c r="B22" s="27"/>
+      <c r="C22" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="D22" s="15"/>
       <c r="F22" t="s">
@@ -2430,44 +2402,32 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="33"/>
-      <c r="B23" s="21"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D23" s="15"/>
       <c r="F23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="34"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="F24" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A20:A24"/>
+  <mergeCells count="14">
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2476,10 +2436,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2490,7 +2450,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="30" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -2500,87 +2460,83 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="28"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="9"/>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="9"/>
+      <c r="A3" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="10"/>
       <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="10"/>
-      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.25">
+      <c r="A4" s="23" t="s">
         <v>41</v>
       </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="13"/>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="17.25">
-      <c r="A5" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="13"/>
       <c r="F5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17.25">
-      <c r="A6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18">
+      <c r="A6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="13"/>
       <c r="F6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="13"/>
-      <c r="F7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17.25">
-      <c r="A8" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="13" t="s">
-        <v>24</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.25">
+      <c r="A7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="F8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D9" s="11"/>
       <c r="F9" t="s">
@@ -2591,144 +2547,144 @@
       <c r="A10" s="3"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" s="11"/>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="D11" s="11"/>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="D12" s="11"/>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D13" s="11"/>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="F14" t="s">
-        <v>54</v>
+      <c r="A14" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="14"/>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="14"/>
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="12"/>
       <c r="F15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="31"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="29"/>
       <c r="D16" s="12"/>
-      <c r="F16" s="1" t="s">
-        <v>25</v>
+      <c r="F16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3"/>
       <c r="B17" s="29" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="12"/>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
       <c r="B18" s="29" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="12"/>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="29"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="D19" s="12"/>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="32"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D20" s="12"/>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="33"/>
-      <c r="B21" s="21"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D21" s="12"/>
       <c r="F21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="33"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="7" t="s">
-        <v>76</v>
+      <c r="B22" s="27"/>
+      <c r="C22" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="D22" s="12"/>
       <c r="F22" t="s">
@@ -2736,44 +2692,32 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="33"/>
-      <c r="B23" s="21"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D23" s="12"/>
       <c r="F23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="34"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="F24" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A6:C6"/>
+  <mergeCells count="14">
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B19:B23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2782,10 +2726,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2794,82 +2738,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="F2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="9"/>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="9"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="39"/>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="41"/>
       <c r="F4" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="12"/>
-      <c r="F5" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="12"/>
-      <c r="F6" t="s">
-        <v>62</v>
+      <c r="A5" s="36"/>
+      <c r="B5" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="42"/>
+      <c r="D5" s="41"/>
+      <c r="F5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A3:C3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2878,10 +2806,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2890,113 +2818,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="A1" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="9"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="39"/>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="36"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="36"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="9"/>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="10"/>
-      <c r="F4" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="44"/>
       <c r="F5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="11"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="41"/>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="35"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="12"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="41"/>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="36"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="12"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="41"/>
       <c r="F8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="37"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="F9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A6:A8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>